<commit_message>
add enemy in battle ui
</commit_message>
<xml_diff>
--- a/Table/main.xlsx
+++ b/Table/main.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>__workbook__</t>
   </si>
@@ -92,14 +92,6 @@
   </si>
   <si>
     <t>Table_Itemcombine</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Table_Enemy1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Enemy/TABLE_Enemy1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -509,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -528,7 +520,7 @@
     <col min="12" max="12" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="19">
+    <row r="1" spans="1:11" ht="19">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -562,63 +554,55 @@
       <c r="K1" t="s">
         <v>19</v>
       </c>
-      <c r="L1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="A12" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>